<commit_message>
Test cases for signup module added
</commit_message>
<xml_diff>
--- a/Login_TestCases.xlsx
+++ b/Login_TestCases.xlsx
@@ -1362,14 +1362,14 @@
   <sheetPr/>
   <dimension ref="A1:N12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="16.7777777777778" customWidth="1"/>
-    <col min="2" max="2" width="32" customWidth="1"/>
+    <col min="2" max="2" width="36.2222222222222" customWidth="1"/>
     <col min="3" max="3" width="12.1111111111111" customWidth="1"/>
     <col min="4" max="4" width="38.5555555555556" customWidth="1"/>
     <col min="5" max="5" width="26.5555555555556" customWidth="1"/>

</xml_diff>